<commit_message>
update jumlah pasien corona 29/3/20
</commit_message>
<xml_diff>
--- a/Data Perkembangan Kasus Corona Indonesia.xlsx
+++ b/Data Perkembangan Kasus Corona Indonesia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Dataset Corona\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Dataset Corona\covid19Indonesia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75326151-5295-4FFF-AC86-683271B39798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5669F72-CC9E-4499-8AC9-B49ADE6DB477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E19278CD-A438-4185-A26E-59B831A71B06}"/>
   </bookViews>
@@ -111,7 +111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -147,11 +147,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -182,6 +193,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774F75F7-5486-4AF2-8B96-271209FEC6DA}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J27" si="0">I3/D3</f>
+        <f t="shared" ref="J3:J29" si="0">I3/D3</f>
         <v>0</v>
       </c>
       <c r="K3" s="3">
@@ -1651,6 +1668,89 @@
       </c>
       <c r="M27" s="3">
         <v>4729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>43918</v>
+      </c>
+      <c r="C28" s="3">
+        <v>109</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1155</v>
+      </c>
+      <c r="E28" s="3">
+        <v>994</v>
+      </c>
+      <c r="F28" s="3">
+        <v>13</v>
+      </c>
+      <c r="G28" s="3">
+        <v>59</v>
+      </c>
+      <c r="H28" s="3">
+        <v>15</v>
+      </c>
+      <c r="I28" s="3">
+        <v>102</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="0"/>
+        <v>8.8311688311688313E-2</v>
+      </c>
+      <c r="K28" s="11">
+        <v>6266</v>
+      </c>
+      <c r="L28" s="11">
+        <v>1155</v>
+      </c>
+      <c r="M28" s="11">
+        <v>5111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>43919</v>
+      </c>
+      <c r="C29">
+        <v>130</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1285</v>
+      </c>
+      <c r="F29" s="11">
+        <v>5</v>
+      </c>
+      <c r="G29" s="11">
+        <v>64</v>
+      </c>
+      <c r="H29" s="11">
+        <v>12</v>
+      </c>
+      <c r="I29" s="11">
+        <v>114</v>
+      </c>
+      <c r="J29" s="12">
+        <f t="shared" si="0"/>
+        <v>8.8715953307393E-2</v>
+      </c>
+      <c r="L29" s="11">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>43920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>